<commit_message>
update email with text shit
</commit_message>
<xml_diff>
--- a/EmailBlast/Excel/Tycadome/Continent/Africa/Ghana.xlsx
+++ b/EmailBlast/Excel/Tycadome/Continent/Africa/Ghana.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\Robots\Ruby\EmailBlast\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\Tech\Software Programming and Coding\Robots\Ruby\EmailBlast\Excel\Tycadome\Continent\Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C294D3-AB70-4CAE-B08B-565D419FA99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E911E3C-F44E-4033-9D0B-B94F1DE08997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" firstSheet="6" activeTab="8" xr2:uid="{A137CB90-262B-4B90-B2EF-3C03DE4DEFB2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="8" xr2:uid="{A137CB90-262B-4B90-B2EF-3C03DE4DEFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrumental" sheetId="1" r:id="rId1"/>

</xml_diff>